<commit_message>
Asset List update & Uren Registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="214">
   <si>
     <t>ID Code</t>
   </si>
@@ -641,6 +641,24 @@
   </si>
   <si>
     <t>F_Pi_01</t>
+  </si>
+  <si>
+    <t>J. UI Design</t>
+  </si>
+  <si>
+    <t>Menu Design | In game Design |</t>
+  </si>
+  <si>
+    <t>J_IGD_01</t>
+  </si>
+  <si>
+    <t>J_MD_01</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>UI Design</t>
   </si>
 </sst>
 </file>
@@ -671,7 +689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,6 +755,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -751,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,6 +828,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -1118,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J362" sqref="J362"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G373" sqref="G373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,6 +1493,9 @@
       <c r="E11" s="1">
         <v>3</v>
       </c>
+      <c r="G11" s="20" t="s">
+        <v>213</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
         <v>27</v>
@@ -1779,9 +1810,15 @@
       <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
+      <c r="H22" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
       <c r="M22"/>
       <c r="N22"/>
       <c r="O22"/>
@@ -7285,6 +7322,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A378" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B378" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E378" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A379" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B379" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E379" s="4">
+        <v>6</v>
+      </c>
+    </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384"/>
       <c r="B384"/>

</xml_diff>

<commit_message>
Scrums and other shit
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>